<commit_message>
RDM-9338: renamed NoCConfig tab to NoticeOfChangeConfig
</commit_message>
<xml_diff>
--- a/aat/src/resource/CCD_CNP_27_CaseType_Invalid_Case_Type_NoC_Config.xlsx
+++ b/aat/src/resource/CCD_CNP_27_CaseType_Invalid_Case_Type_NoC_Config.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kiranyenigala/Projects/CCD/ccd-definition-store-api/aat/src/resource/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36C6A3E0-16BF-AB48-9235-90C8CD2E3B7E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68F611A7-15B3-B341-8BF2-427B36001C03}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1080" windowWidth="29180" windowHeight="16620" tabRatio="823" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
     <sheet name="CaseType" sheetId="2" r:id="rId2"/>
-    <sheet name="NoCConfig" sheetId="20" r:id="rId3"/>
+    <sheet name="NoticeOfChangeConfig" sheetId="20" r:id="rId3"/>
     <sheet name="CaseField" sheetId="3" r:id="rId4"/>
     <sheet name="FixedLists" sheetId="4" r:id="rId5"/>
     <sheet name="ComplexTypes" sheetId="5" r:id="rId6"/>
@@ -904,9 +904,6 @@
     <t>caseworker-autotest1</t>
   </si>
   <si>
-    <t>NoCConfig</t>
-  </si>
-  <si>
     <t>CaseTypeId</t>
   </si>
   <si>
@@ -929,6 +926,9 @@
   </si>
   <si>
     <t>AATPUBLIC1</t>
+  </si>
+  <si>
+    <t>NoticeOfChangeConfig</t>
   </si>
 </sst>
 </file>
@@ -1732,13 +1732,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="thin">
           <color rgb="FF000000"/>
         </left>
@@ -1773,6 +1766,13 @@
         </patternFill>
       </fill>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -1824,7 +1824,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{14A5C809-B9D9-A84A-8C45-06D62D4C0E7F}" name="Table414" displayName="Table414" ref="A3:C7" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6" headerRowBorderDxfId="4" tableBorderDxfId="5" totalsRowBorderDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{14A5C809-B9D9-A84A-8C45-06D62D4C0E7F}" name="Table414" displayName="Table414" ref="A3:C7" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4" totalsRowBorderDxfId="3">
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{E1E30C7A-98C1-564B-9792-5DF60A18DC40}" name="CaseTypeId" dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{CF132C8A-FB04-6E49-A4E6-6E1D8EB03DA6}" name="ReasonRequired" dataDxfId="1"/>
@@ -6635,7 +6635,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -6647,42 +6647,42 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="87" t="s">
-        <v>280</v>
+        <v>288</v>
       </c>
       <c r="B1" s="88"/>
       <c r="C1" s="88"/>
     </row>
-    <row r="2" spans="1:3" ht="84" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:3" ht="28" x14ac:dyDescent="0.15">
       <c r="A2" s="89" t="s">
+        <v>280</v>
+      </c>
+      <c r="B2" s="89" t="s">
         <v>281</v>
       </c>
-      <c r="B2" s="89" t="s">
+      <c r="C2" s="89" t="s">
         <v>282</v>
-      </c>
-      <c r="C2" s="89" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.15">
       <c r="A3" s="90" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B3" s="91" t="s">
+        <v>283</v>
+      </c>
+      <c r="C3" s="92" t="s">
         <v>284</v>
-      </c>
-      <c r="C3" s="92" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="18" x14ac:dyDescent="0.15">
       <c r="A4" s="93" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B4" s="93" t="s">
+        <v>285</v>
+      </c>
+      <c r="C4" s="94" t="s">
         <v>286</v>
-      </c>
-      <c r="C4" s="94" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="18" x14ac:dyDescent="0.15">

</xml_diff>